<commit_message>
Completed my EDA using a REGEX
</commit_message>
<xml_diff>
--- a/CH-149 Extract From Text.xlsx
+++ b/CH-149 Extract From Text.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FFFD3C8-8A47-490C-9021-14FE2548E9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AEA123-59D5-4AC7-8CCB-6A217F1556D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +40,45 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -379,8 +418,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>43963</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>36634</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23446</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -395,8 +434,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="249117" y="1707173"/>
-          <a:ext cx="4637942" cy="930519"/>
+          <a:off x="241791" y="1504950"/>
+          <a:ext cx="4632080" cy="1261696"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -522,6 +561,65 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <fb t="e">#N/A</fb>
+    <v>6</v>
+    <v>9</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -802,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -933,4 +1031,175 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CEF490B-38AD-482D-B577-4AF5D3F34C16}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="44" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.3984375" customWidth="1"/>
+    <col min="4" max="4" width="11.8984375" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="str" cm="1">
+        <f t="array" ref="B13:B17">_xlfn.REGEXEXTRACT(B3:B7,"\(([^)]+)\)|\[([^]]+)\]|\{([^}]+)\}",2,1)</f>
+        <v>quick brown</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5" t="str" cm="1">
+        <f t="array" ref="D13:D17">_xlfn.MAP(B3:B7,_xlfn.LAMBDA(_xlpm.x,_xlfn.TEXTJOIN("",1,_xlfn.IFNA(_xlfn.REGEXEXTRACT(_xlpm.x,"\(([^)]+)\)|\[([^]]+)\]|\{([^}]+)\}",2,1),""))))</f>
+        <v>quick brown</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="e" vm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <v>reading books</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="e" vm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <v>beach for</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="str">
+        <v>chocolate cake</v>
+      </c>
+      <c r="D16" s="5" t="str">
+        <v>chocolate cake</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="e" vm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <v>playing guitar</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Got first Alt working
</commit_message>
<xml_diff>
--- a/CH-149 Extract From Text.xlsx
+++ b/CH-149 Extract From Text.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AEA123-59D5-4AC7-8CCB-6A217F1556D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DED59FD-4148-43CC-A448-C396B90DC686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt1 (2)" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt1 (2)'!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$13</definedName>
   </definedNames>
@@ -78,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -1037,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CEF490B-38AD-482D-B577-4AF5D3F34C16}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1202,4 +1206,302 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AE1FF0-406B-4912-A3F1-E05204099246}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="44" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.3984375" customWidth="1"/>
+    <col min="4" max="4" width="11.8984375" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="str" cm="1">
+        <f t="array" ref="B11:B15">_xlfn.REGEXEXTRACT(B3:B7, "(?&lt;=\{)[^}]*|(?&lt;=\[)[^\]]*|(?&lt;=\()[^)]*")</f>
+        <v>quick brown</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="str">
+        <v>reading books</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="str">
+        <v>beach for</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="str">
+        <v>chocolate cake</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="str">
+        <v>playing guitar</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0567F1CF-FBE0-49EE-8B3F-A8AFE61BD0AE}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="44" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.3984375" customWidth="1"/>
+    <col min="4" max="4" width="11.8984375" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="str" cm="1">
+        <f t="array" ref="B11:B15">_xlfn.REGEXEXTRACT(B3:B7, "(?&lt;=\{)[^}]*|(?&lt;=\[)[^\]]*|(?&lt;=\()[^)]*")</f>
+        <v>quick brown</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="str">
+        <v>reading books</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="str">
+        <v>beach for</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="str">
+        <v>chocolate cake</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="str">
+        <v>playing guitar</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Got 2nd Alt working
</commit_message>
<xml_diff>
--- a/CH-149 Extract From Text.xlsx
+++ b/CH-149 Extract From Text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DED59FD-4148-43CC-A448-C396B90DC686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92337884-3605-4D50-B59E-7ABBF4CF7DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,11 @@
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
-    <sheet name="Alt1 (2)" sheetId="4" r:id="rId4"/>
+    <sheet name="Alt2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$C$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt1 (2)'!$B$2:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$13</definedName>
   </definedNames>
@@ -1362,7 +1362,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str" cm="1">
-        <f t="array" ref="B11:B15">_xlfn.REGEXEXTRACT(B3:B7, "(?&lt;=\{)[^}]*|(?&lt;=\[)[^\]]*|(?&lt;=\()[^)]*")</f>
+        <f t="array" ref="B11:B15">_xlfn.BYROW(B3:B7,_xlfn.LAMBDA(_xlpm.x,_xlfn.REGEXEXTRACT(_xlpm.x,"(?&lt;=\().*?(?=\))|(?&lt;=\[).*?(?=\])|(?&lt;=\{).*?(?=\})")))</f>
         <v>quick brown</v>
       </c>
       <c r="C11" s="7"/>

</xml_diff>

<commit_message>
Got 3rd Alt (no regex) working
</commit_message>
<xml_diff>
--- a/CH-149 Extract From Text.xlsx
+++ b/CH-149 Extract From Text.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92337884-3605-4D50-B59E-7ABBF4CF7DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5054A2-694F-41EA-A682-2D7B23068C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="4" r:id="rId4"/>
+    <sheet name="Alt3" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt3'!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$13</definedName>
   </definedNames>
@@ -82,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="15">
   <si>
     <t>Question</t>
   </si>
@@ -146,6 +148,9 @@
       </rPr>
       <t>) was delicious and rich.</t>
     </r>
+  </si>
+  <si>
+    <t>No Regex</t>
   </si>
 </sst>
 </file>
@@ -1361,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0567F1CF-FBE0-49EE-8B3F-A8AFE61BD0AE}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1504,4 +1509,155 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D821238-2373-46B2-88E8-DA90725ABA2C}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="44" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.3984375" customWidth="1"/>
+    <col min="4" max="4" width="11.8984375" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="str" cm="1">
+        <f t="array" ref="B11:B15">_xlfn.MAP(B3:B7,_xlfn.LAMBDA(_xlpm.x,INDEX(_xlfn.TEXTSPLIT(_xlpm.x,{"(",")","[","]","{","}"}),,2)))</f>
+        <v>quick brown</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="str">
+        <v>reading books</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="str">
+        <v>beach for</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="str">
+        <v>chocolate cake</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="str">
+        <v>playing guitar</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
The non-regex is pretty clever
</commit_message>
<xml_diff>
--- a/CH-149 Extract From Text.xlsx
+++ b/CH-149 Extract From Text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5054A2-694F-41EA-A682-2D7B23068C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C07C47-57AA-4E71-B9F2-4F28C36D4926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1516,7 +1516,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1633,27 +1633,77 @@
         <v>quick brown</v>
       </c>
       <c r="C11" s="7"/>
+      <c r="D11" s="5" t="str" cm="1">
+        <f t="array" ref="D11:F11">_xlfn.TEXTSPLIT(B3,{"(",")","[","]","{","}"})</f>
+        <v xml:space="preserve">The </v>
+      </c>
+      <c r="E11" t="str">
+        <v>quick brown</v>
+      </c>
+      <c r="F11" t="str">
+        <v xml:space="preserve"> fox jumps over the lazy dog.</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="str">
         <v>reading books</v>
       </c>
       <c r="C12" s="7"/>
+      <c r="D12" s="5" t="str" cm="1">
+        <f t="array" ref="D12:F12">_xlfn.TEXTSPLIT(B4,{"(",")","[","]","{","}"})</f>
+        <v xml:space="preserve">She enjoys </v>
+      </c>
+      <c r="E12" t="str">
+        <v>reading books</v>
+      </c>
+      <c r="F12" t="str">
+        <v xml:space="preserve"> on rainy days.</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str">
         <v>beach for</v>
       </c>
       <c r="C13" s="7"/>
+      <c r="D13" s="5" t="str" cm="1">
+        <f t="array" ref="D13:F13">_xlfn.TEXTSPLIT(B5,{"(",")","[","]","{","}"})</f>
+        <v xml:space="preserve">They went to the </v>
+      </c>
+      <c r="E13" t="str">
+        <v>beach for</v>
+      </c>
+      <c r="F13" t="str">
+        <v xml:space="preserve"> a fun weekend.</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="str">
         <v>chocolate cake</v>
       </c>
+      <c r="D14" s="5" t="str" cm="1">
+        <f t="array" ref="D14:F14">_xlfn.TEXTSPLIT(B6,{"(",")","[","]","{","}"})</f>
+        <v xml:space="preserve">The </v>
+      </c>
+      <c r="E14" t="str">
+        <v>chocolate cake</v>
+      </c>
+      <c r="F14" t="str">
+        <v xml:space="preserve"> was delicious and rich.</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <v>playing guitar</v>
+      </c>
+      <c r="D15" s="5" t="str" cm="1">
+        <f t="array" ref="D15:F15">_xlfn.TEXTSPLIT(B7,{"(",")","[","]","{","}"})</f>
+        <v xml:space="preserve">He loves </v>
+      </c>
+      <c r="E15" t="str">
+        <v>playing guitar</v>
+      </c>
+      <c r="F15" t="str">
+        <v xml:space="preserve"> in his free time.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Another wack at understanding the grouping problem
</commit_message>
<xml_diff>
--- a/CH-149 Extract From Text.xlsx
+++ b/CH-149 Extract From Text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C07C47-57AA-4E71-B9F2-4F28C36D4926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6379CF-A179-4083-9D11-B2BF70895F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AE1FF0-406B-4912-A3F1-E05204099246}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1227,6 +1227,7 @@
     <col min="2" max="2" width="44" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.3984375" customWidth="1"/>
     <col min="4" max="4" width="11.8984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1333,26 +1334,42 @@
         <v>quick brown</v>
       </c>
       <c r="C11" s="7"/>
+      <c r="F11" t="str" cm="1">
+        <f t="array" ref="F11:F15">_xlfn.MAP(B3:B7,_xlfn.LAMBDA(_xlpm.x, _xlfn.CONCAT(_xlfn.IFNA(_xlfn.REGEXEXTRACT(_xlpm.x,"\((.*)\)|\[(.*)\]|\{(.*)\}",2,1),""))))</f>
+        <v>quick brown</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="str">
         <v>reading books</v>
       </c>
       <c r="C12" s="7"/>
+      <c r="F12" t="str">
+        <v>reading books</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str">
         <v>beach for</v>
       </c>
       <c r="C13" s="7"/>
+      <c r="F13" t="str">
+        <v>beach for</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="str">
         <v>chocolate cake</v>
       </c>
+      <c r="F14" t="str">
+        <v>chocolate cake</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
+        <v>playing guitar</v>
+      </c>
+      <c r="F15" t="str">
         <v>playing guitar</v>
       </c>
     </row>
@@ -1515,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D821238-2373-46B2-88E8-DA90725ABA2C}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>